<commit_message>
Run with K_S ~ HalfFlat
</commit_message>
<xml_diff>
--- a/data_and_analysis/processed/full_parameter_mapping.xlsx
+++ b/data_and_analysis/processed/full_parameter_mapping.xlsx
@@ -486,8 +486,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>0.02</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -516,8 +518,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>0.02</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -546,8 +550,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>0.02</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -576,8 +582,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>0.02</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -606,8 +614,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>0.02</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -636,8 +646,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>0.02</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -666,8 +678,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>0.02</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -696,8 +710,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>0.02</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -726,8 +742,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>0.02</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -756,8 +774,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>0.02</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -786,8 +806,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E12" t="n">
-        <v>0.02</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -816,8 +838,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>0.02</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -846,8 +870,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>0.02</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -876,8 +902,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>0.02</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -906,8 +934,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E16" t="n">
-        <v>0.02</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -936,8 +966,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E17" t="n">
-        <v>0.02</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -966,8 +998,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E18" t="n">
-        <v>0.02</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -996,8 +1030,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E19" t="n">
-        <v>0.02</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1026,8 +1062,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E20" t="n">
-        <v>0.02</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1056,8 +1094,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>0.02</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1086,8 +1126,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E22" t="n">
-        <v>0.02</v>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1116,8 +1158,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E23" t="n">
-        <v>0.02</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1146,8 +1190,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E24" t="n">
-        <v>0.02</v>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1176,8 +1222,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E25" t="n">
-        <v>0.02</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1206,8 +1254,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E26" t="n">
-        <v>0.02</v>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1236,8 +1286,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>0.02</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1266,8 +1318,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E28" t="n">
-        <v>0.02</v>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1296,8 +1350,10 @@
           <t>mu_max</t>
         </is>
       </c>
-      <c r="E29" t="n">
-        <v>0.02</v>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>K_S</t>
+        </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>

</xml_diff>